<commit_message>
update: hw02 has the g ones selected
Signed-off-by: the-other-mariana <mariana.avalos.arce@gmail.com>
</commit_message>
<xml_diff>
--- a/PM2/econ/week5/hw2_MarianaAvalos.xlsx
+++ b/PM2/econ/week5/hw2_MarianaAvalos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mariana\Documents\github-mariana\pm\PM2\econ\week5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AF58F5F-572C-4287-BA6E-D39CE2044E6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8A16ED5-A946-42A9-B909-561B47C0680E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="8" xr2:uid="{9F559EE0-24DC-4C0C-8898-02AA049EDE74}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="8" activeTab="24" xr2:uid="{9F559EE0-24DC-4C0C-8898-02AA049EDE74}"/>
   </bookViews>
   <sheets>
     <sheet name="ex1" sheetId="1" r:id="rId1"/>
@@ -18,26 +18,26 @@
     <sheet name="ex3" sheetId="3" r:id="rId3"/>
     <sheet name="ex4" sheetId="4" r:id="rId4"/>
     <sheet name="ex5" sheetId="5" r:id="rId5"/>
-    <sheet name="ex6" sheetId="6" r:id="rId6"/>
-    <sheet name="ex7" sheetId="7" r:id="rId7"/>
+    <sheet name="ex6g" sheetId="6" r:id="rId6"/>
+    <sheet name="ex7g" sheetId="7" r:id="rId7"/>
     <sheet name="ex8" sheetId="8" r:id="rId8"/>
     <sheet name="ex9d" sheetId="9" r:id="rId9"/>
     <sheet name="ex10" sheetId="10" r:id="rId10"/>
     <sheet name="ex11" sheetId="11" r:id="rId11"/>
-    <sheet name="ex12d" sheetId="12" r:id="rId12"/>
+    <sheet name="ex12dg" sheetId="12" r:id="rId12"/>
     <sheet name="ex13" sheetId="13" r:id="rId13"/>
     <sheet name="ex14" sheetId="14" r:id="rId14"/>
-    <sheet name="ex15d" sheetId="15" r:id="rId15"/>
+    <sheet name="ex15dg" sheetId="15" r:id="rId15"/>
     <sheet name="ex16" sheetId="16" r:id="rId16"/>
     <sheet name="ex17" sheetId="17" r:id="rId17"/>
     <sheet name="ex18d" sheetId="18" r:id="rId18"/>
     <sheet name="ex19" sheetId="19" r:id="rId19"/>
     <sheet name="ex20" sheetId="20" r:id="rId20"/>
-    <sheet name="ex21d" sheetId="21" r:id="rId21"/>
+    <sheet name="ex21dg" sheetId="21" r:id="rId21"/>
     <sheet name="ex22" sheetId="22" r:id="rId22"/>
     <sheet name="ex23d" sheetId="23" r:id="rId23"/>
-    <sheet name="ex24" sheetId="24" r:id="rId24"/>
-    <sheet name="ex25" sheetId="25" r:id="rId25"/>
+    <sheet name="ex24g" sheetId="24" r:id="rId24"/>
+    <sheet name="ex25g" sheetId="25" r:id="rId25"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="423" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="101">
   <si>
     <t>Flujo</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t xml:space="preserve">Por lo tanto, a menos q el gasto anual sea igual a la inversión inicial, siempre conviene la opción barata </t>
+  </si>
+  <si>
+    <t>si la TIR es mayor q el costo de op, realmente importa cuánto?</t>
   </si>
 </sst>
 </file>
@@ -661,7 +664,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>ex15d!$B$30:$AE$30</c:f>
+              <c:f>ex15dg!$B$30:$AE$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -760,7 +763,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ex15d!$B$31:$AE$31</c:f>
+              <c:f>ex15dg!$B$31:$AE$31</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -884,7 +887,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>ex15d!$B$32:$AE$32</c:f>
+              <c:f>ex15dg!$B$32:$AE$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -1303,7 +1306,7 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>ex15d!$A$40:$A$59</c:f>
+              <c:f>ex15dg!$A$40:$A$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -1372,7 +1375,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>ex15d!$B$40:$B$59</c:f>
+              <c:f>ex15dg!$B$40:$B$59</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
@@ -4694,7 +4697,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE71B3D-07DB-403D-B078-251ACAEB728E}">
   <dimension ref="A10:F20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
@@ -4901,8 +4904,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA64920-31ED-4322-8AF2-7FC8CD0FFC72}">
   <dimension ref="A10:K20"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:K20"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5243,10 +5246,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7DBC4EE4-AA93-4AEF-A565-63F12DD2D796}">
-  <dimension ref="B6:I17"/>
+  <dimension ref="B6:I20"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5465,6 +5468,11 @@
       <c r="H17">
         <f>F17/C15</f>
         <v>-0.65306122448979576</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -6336,8 +6344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{675E4367-2A6A-4CD7-9D9C-9C5B4CDF4F9C}">
   <dimension ref="A14:AE59"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K54" sqref="K54"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6845,119 +6853,119 @@
         <v>-3184.9327231746461</v>
       </c>
       <c r="C31">
-        <f>C30+(C30*$A$30)/(1+$A$24)^(1)+(C30*$A$30)/(1+$A$24)^(2)+(C30*$A$30)/(1+$A$24)^(3)+(C30*$A$30)/(1+$A$24)^(4)+(C30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" ref="B31:AE31" si="9">C30+(C30*$A$30)/(1+$A$24)^(1)+(C30*$A$30)/(1+$A$24)^(2)+(C30*$A$30)/(1+$A$24)^(3)+(C30*$A$30)/(1+$A$24)^(4)+(C30*$A$30)/(1+$A$24)^(5)</f>
         <v>-3474.4720616450686</v>
       </c>
       <c r="D31">
-        <f>D30+(D30*$A$30)/(1+$A$24)^(1)+(D30*$A$30)/(1+$A$24)^(2)+(D30*$A$30)/(1+$A$24)^(3)+(D30*$A$30)/(1+$A$24)^(4)+(D30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-3764.0114001154911</v>
       </c>
       <c r="E31">
-        <f>E30+(E30*$A$30)/(1+$A$24)^(1)+(E30*$A$30)/(1+$A$24)^(2)+(E30*$A$30)/(1+$A$24)^(3)+(E30*$A$30)/(1+$A$24)^(4)+(E30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-4053.5507385859137</v>
       </c>
       <c r="F31">
-        <f>F30+(F30*$A$30)/(1+$A$24)^(1)+(F30*$A$30)/(1+$A$24)^(2)+(F30*$A$30)/(1+$A$24)^(3)+(F30*$A$30)/(1+$A$24)^(4)+(F30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-4343.0900770563358</v>
       </c>
       <c r="G31">
-        <f>G30+(G30*$A$30)/(1+$A$24)^(1)+(G30*$A$30)/(1+$A$24)^(2)+(G30*$A$30)/(1+$A$24)^(3)+(G30*$A$30)/(1+$A$24)^(4)+(G30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-4632.6294155267578</v>
       </c>
       <c r="H31">
-        <f>H30+(H30*$A$30)/(1+$A$24)^(1)+(H30*$A$30)/(1+$A$24)^(2)+(H30*$A$30)/(1+$A$24)^(3)+(H30*$A$30)/(1+$A$24)^(4)+(H30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-4922.1687539971799</v>
       </c>
       <c r="I31">
-        <f>I30+(I30*$A$30)/(1+$A$24)^(1)+(I30*$A$30)/(1+$A$24)^(2)+(I30*$A$30)/(1+$A$24)^(3)+(I30*$A$30)/(1+$A$24)^(4)+(I30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-5211.7080924676029</v>
       </c>
       <c r="J31">
-        <f>J30+(J30*$A$30)/(1+$A$24)^(1)+(J30*$A$30)/(1+$A$24)^(2)+(J30*$A$30)/(1+$A$24)^(3)+(J30*$A$30)/(1+$A$24)^(4)+(J30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-5501.247430938025</v>
       </c>
       <c r="K31">
-        <f>K30+(K30*$A$30)/(1+$A$24)^(1)+(K30*$A$30)/(1+$A$24)^(2)+(K30*$A$30)/(1+$A$24)^(3)+(K30*$A$30)/(1+$A$24)^(4)+(K30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-5790.7867694084471</v>
       </c>
       <c r="L31">
-        <f>L30+(L30*$A$30)/(1+$A$24)^(1)+(L30*$A$30)/(1+$A$24)^(2)+(L30*$A$30)/(1+$A$24)^(3)+(L30*$A$30)/(1+$A$24)^(4)+(L30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-6080.3261078788701</v>
       </c>
       <c r="M31">
-        <f>M30+(M30*$A$30)/(1+$A$24)^(1)+(M30*$A$30)/(1+$A$24)^(2)+(M30*$A$30)/(1+$A$24)^(3)+(M30*$A$30)/(1+$A$24)^(4)+(M30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-6369.8654463492921</v>
       </c>
       <c r="N31">
-        <f>N30+(N30*$A$30)/(1+$A$24)^(1)+(N30*$A$30)/(1+$A$24)^(2)+(N30*$A$30)/(1+$A$24)^(3)+(N30*$A$30)/(1+$A$24)^(4)+(N30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-6659.4047848197142</v>
       </c>
       <c r="O31">
-        <f>O30+(O30*$A$30)/(1+$A$24)^(1)+(O30*$A$30)/(1+$A$24)^(2)+(O30*$A$30)/(1+$A$24)^(3)+(O30*$A$30)/(1+$A$24)^(4)+(O30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-6948.9441232901372</v>
       </c>
       <c r="P31">
-        <f>P30+(P30*$A$30)/(1+$A$24)^(1)+(P30*$A$30)/(1+$A$24)^(2)+(P30*$A$30)/(1+$A$24)^(3)+(P30*$A$30)/(1+$A$24)^(4)+(P30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-7238.4834617605602</v>
       </c>
       <c r="Q31">
-        <f>Q30+(Q30*$A$30)/(1+$A$24)^(1)+(Q30*$A$30)/(1+$A$24)^(2)+(Q30*$A$30)/(1+$A$24)^(3)+(Q30*$A$30)/(1+$A$24)^(4)+(Q30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-7528.0228002309823</v>
       </c>
       <c r="R31">
-        <f>R30+(R30*$A$30)/(1+$A$24)^(1)+(R30*$A$30)/(1+$A$24)^(2)+(R30*$A$30)/(1+$A$24)^(3)+(R30*$A$30)/(1+$A$24)^(4)+(R30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-7817.5621387014044</v>
       </c>
       <c r="S31">
-        <f>S30+(S30*$A$30)/(1+$A$24)^(1)+(S30*$A$30)/(1+$A$24)^(2)+(S30*$A$30)/(1+$A$24)^(3)+(S30*$A$30)/(1+$A$24)^(4)+(S30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-8107.1014771718274</v>
       </c>
       <c r="T31">
-        <f>T30+(T30*$A$30)/(1+$A$24)^(1)+(T30*$A$30)/(1+$A$24)^(2)+(T30*$A$30)/(1+$A$24)^(3)+(T30*$A$30)/(1+$A$24)^(4)+(T30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-8396.6408156422476</v>
       </c>
       <c r="U31">
-        <f>U30+(U30*$A$30)/(1+$A$24)^(1)+(U30*$A$30)/(1+$A$24)^(2)+(U30*$A$30)/(1+$A$24)^(3)+(U30*$A$30)/(1+$A$24)^(4)+(U30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-8686.1801541126715</v>
       </c>
       <c r="V31">
-        <f>V30+(V30*$A$30)/(1+$A$24)^(1)+(V30*$A$30)/(1+$A$24)^(2)+(V30*$A$30)/(1+$A$24)^(3)+(V30*$A$30)/(1+$A$24)^(4)+(V30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-8975.7194925830936</v>
       </c>
       <c r="W31">
-        <f>W30+(W30*$A$30)/(1+$A$24)^(1)+(W30*$A$30)/(1+$A$24)^(2)+(W30*$A$30)/(1+$A$24)^(3)+(W30*$A$30)/(1+$A$24)^(4)+(W30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-9265.2588310535157</v>
       </c>
       <c r="X31">
-        <f>X30+(X30*$A$30)/(1+$A$24)^(1)+(X30*$A$30)/(1+$A$24)^(2)+(X30*$A$30)/(1+$A$24)^(3)+(X30*$A$30)/(1+$A$24)^(4)+(X30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-9554.7981695239378</v>
       </c>
       <c r="Y31">
-        <f>Y30+(Y30*$A$30)/(1+$A$24)^(1)+(Y30*$A$30)/(1+$A$24)^(2)+(Y30*$A$30)/(1+$A$24)^(3)+(Y30*$A$30)/(1+$A$24)^(4)+(Y30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-9844.3375079943598</v>
       </c>
       <c r="Z31">
-        <f>Z30+(Z30*$A$30)/(1+$A$24)^(1)+(Z30*$A$30)/(1+$A$24)^(2)+(Z30*$A$30)/(1+$A$24)^(3)+(Z30*$A$30)/(1+$A$24)^(4)+(Z30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-10133.876846464784</v>
       </c>
       <c r="AA31">
-        <f>AA30+(AA30*$A$30)/(1+$A$24)^(1)+(AA30*$A$30)/(1+$A$24)^(2)+(AA30*$A$30)/(1+$A$24)^(3)+(AA30*$A$30)/(1+$A$24)^(4)+(AA30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-10423.416184935206</v>
       </c>
       <c r="AB31">
-        <f>AB30+(AB30*$A$30)/(1+$A$24)^(1)+(AB30*$A$30)/(1+$A$24)^(2)+(AB30*$A$30)/(1+$A$24)^(3)+(AB30*$A$30)/(1+$A$24)^(4)+(AB30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-10712.955523405628</v>
       </c>
       <c r="AC31">
-        <f>AC30+(AC30*$A$30)/(1+$A$24)^(1)+(AC30*$A$30)/(1+$A$24)^(2)+(AC30*$A$30)/(1+$A$24)^(3)+(AC30*$A$30)/(1+$A$24)^(4)+(AC30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-11002.49486187605</v>
       </c>
       <c r="AD31">
-        <f>AD30+(AD30*$A$30)/(1+$A$24)^(1)+(AD30*$A$30)/(1+$A$24)^(2)+(AD30*$A$30)/(1+$A$24)^(3)+(AD30*$A$30)/(1+$A$24)^(4)+(AD30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-11292.034200346472</v>
       </c>
       <c r="AE31">
-        <f>AE30+(AE30*$A$30)/(1+$A$24)^(1)+(AE30*$A$30)/(1+$A$24)^(2)+(AE30*$A$30)/(1+$A$24)^(3)+(AE30*$A$30)/(1+$A$24)^(4)+(AE30*$A$30)/(1+$A$24)^(5)</f>
+        <f t="shared" si="9"/>
         <v>-11581.573538816894</v>
       </c>
     </row>
@@ -6966,39 +6974,39 @@
         <v>90</v>
       </c>
       <c r="B32">
-        <f t="shared" ref="B32:J32" si="9">(B30+1000)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(1)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(2)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(3)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(4)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(5)</f>
+        <f t="shared" ref="B32:J32" si="10">(B30+1000)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(1)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(2)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(3)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(4)+(((B30+1000)*$A$30)-333)/(1+$A$24)^(5)</f>
         <v>-1551.8713326834354</v>
       </c>
       <c r="C32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-1841.4106711538579</v>
       </c>
       <c r="D32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2130.95000962428</v>
       </c>
       <c r="E32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2420.4893480947026</v>
       </c>
       <c r="F32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2710.0286865651251</v>
       </c>
       <c r="G32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-2999.5680250355472</v>
       </c>
       <c r="H32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-3289.1073635059693</v>
       </c>
       <c r="I32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-3578.6467019763913</v>
       </c>
       <c r="J32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>-3868.1860404468143</v>
       </c>
       <c r="K32">
@@ -7006,83 +7014,83 @@
         <v>-4157.7253789172364</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32:AE32" si="10">(L30+1000)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(1)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(2)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(3)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(4)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(5)</f>
+        <f t="shared" ref="L32:AE32" si="11">(L30+1000)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(1)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(2)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(3)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(4)+(((L30+1000)*$A$30)-333)/(1+$A$24)^(5)</f>
         <v>-4447.2647173876594</v>
       </c>
       <c r="M32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-4736.8040558580815</v>
       </c>
       <c r="N32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-5026.3433943285036</v>
       </c>
       <c r="O32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-5315.8827327989266</v>
       </c>
       <c r="P32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-5605.4220712693495</v>
       </c>
       <c r="Q32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-5894.9614097397716</v>
       </c>
       <c r="R32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-6184.5007482101937</v>
       </c>
       <c r="S32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-6474.0400866806167</v>
       </c>
       <c r="T32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-6763.5794251510388</v>
       </c>
       <c r="U32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-7053.1187636214618</v>
       </c>
       <c r="V32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-7342.6581020918838</v>
       </c>
       <c r="W32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-7632.1974405623041</v>
       </c>
       <c r="X32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-7921.7367790327271</v>
       </c>
       <c r="Y32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-8211.2761175031501</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-8500.8154559735722</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-8790.3547944439943</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-9079.8941329144182</v>
       </c>
       <c r="AC32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-9369.4334713848402</v>
       </c>
       <c r="AD32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-9658.9728098552623</v>
       </c>
       <c r="AE32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>-9948.5121483256844</v>
       </c>
     </row>
@@ -7095,119 +7103,119 @@
         <v>1633.0613904912107</v>
       </c>
       <c r="C33">
-        <f t="shared" ref="C33:AE33" si="11">ABS(C31)-ABS(C32)</f>
+        <f t="shared" ref="C33:AE33" si="12">ABS(C31)-ABS(C32)</f>
         <v>1633.0613904912107</v>
       </c>
       <c r="D33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912111</v>
       </c>
       <c r="E33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912111</v>
       </c>
       <c r="F33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="G33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="H33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="I33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912116</v>
       </c>
       <c r="J33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="K33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="L33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="M33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="N33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="O33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="P33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="Q33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="R33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="S33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="T33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912088</v>
       </c>
       <c r="U33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
       <c r="V33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
       <c r="W33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912116</v>
       </c>
       <c r="X33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912107</v>
       </c>
       <c r="Y33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912116</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912116</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
       <c r="AC33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
       <c r="AD33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
       <c r="AE33">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1633.0613904912097</v>
       </c>
     </row>
@@ -7267,7 +7275,7 @@
         <v>0.1</v>
       </c>
       <c r="B41">
-        <f t="shared" ref="B41:B59" si="12">1000+(1000*A41-333)/(1+$A$24)^(1)+(1000*A41-333)/(1+$A$24)^(2)+(1000*A41-333)/(1+$A$24)^(3)+(1000*A41-333)/(1+$A$24)^(4)+(1000*A41-333)/(1+$A$24)^(5)</f>
+        <f t="shared" ref="B41:B58" si="13">1000+(1000*A41-333)/(1+$A$24)^(1)+(1000*A41-333)/(1+$A$24)^(2)+(1000*A41-333)/(1+$A$24)^(3)+(1000*A41-333)/(1+$A$24)^(4)+(1000*A41-333)/(1+$A$24)^(5)</f>
         <v>116.7466827278318</v>
       </c>
     </row>
@@ -7276,7 +7284,7 @@
         <v>0.2</v>
       </c>
       <c r="B42">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>495.82535966867641</v>
       </c>
     </row>
@@ -7285,7 +7293,7 @@
         <v>0.3</v>
       </c>
       <c r="B43">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>874.9040366095212</v>
       </c>
     </row>
@@ -7294,7 +7302,7 @@
         <v>0.4</v>
       </c>
       <c r="B44">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1253.9827135503663</v>
       </c>
     </row>
@@ -7303,7 +7311,7 @@
         <v>0.5</v>
       </c>
       <c r="B45">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>1633.0613904912109</v>
       </c>
     </row>
@@ -7312,7 +7320,7 @@
         <v>0.6</v>
       </c>
       <c r="B46">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2012.1400674320555</v>
       </c>
     </row>
@@ -7321,7 +7329,7 @@
         <v>0.7</v>
       </c>
       <c r="B47">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2391.2187443728999</v>
       </c>
     </row>
@@ -7330,7 +7338,7 @@
         <v>0.8</v>
       </c>
       <c r="B48">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>2770.297421313745</v>
       </c>
     </row>
@@ -7339,7 +7347,7 @@
         <v>0.9</v>
       </c>
       <c r="B49">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3149.3760982545896</v>
       </c>
     </row>
@@ -7348,7 +7356,7 @@
         <v>1</v>
       </c>
       <c r="B50">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3528.4547751954342</v>
       </c>
     </row>
@@ -7357,7 +7365,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B51">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>3907.5334521362793</v>
       </c>
     </row>
@@ -7366,7 +7374,7 @@
         <v>1.2</v>
       </c>
       <c r="B52">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4286.6121290771234</v>
       </c>
     </row>
@@ -7375,7 +7383,7 @@
         <v>1.3</v>
       </c>
       <c r="B53">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>4665.6908060179685</v>
       </c>
     </row>
@@ -7384,7 +7392,7 @@
         <v>1.4</v>
       </c>
       <c r="B54">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5044.7694829588127</v>
       </c>
       <c r="D54" t="s">
@@ -7396,7 +7404,7 @@
         <v>1.5</v>
       </c>
       <c r="B55">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5423.8481598996586</v>
       </c>
       <c r="D55" t="s">
@@ -7408,7 +7416,7 @@
         <v>1.6</v>
       </c>
       <c r="B56">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>5802.9268368405028</v>
       </c>
     </row>
@@ -7417,7 +7425,7 @@
         <v>1.7</v>
       </c>
       <c r="B57">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6182.0055137813479</v>
       </c>
     </row>
@@ -7426,7 +7434,7 @@
         <v>1.8</v>
       </c>
       <c r="B58">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>6561.0841907221929</v>
       </c>
     </row>
@@ -7642,7 +7650,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{078CDAC9-A9F9-4F9F-A48B-FF2696E6D7F7}">
   <dimension ref="B10:I33"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
@@ -8026,7 +8034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E52AB25-B78C-4726-B2F8-04AD68AFD30F}">
   <dimension ref="A12:H25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="B7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
@@ -8359,7 +8367,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A2E7DE8-B89D-4BF1-9672-84B2D32A0E78}">
   <dimension ref="A10:K20"/>
   <sheetViews>
-    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -8653,7 +8661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA657E1F-4727-4CE7-94F3-AC92CB58CD41}">
   <dimension ref="A9:H16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -8792,7 +8800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69098D6C-CCF0-4E20-87FA-FD5D71473494}">
   <dimension ref="A11:BC33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
@@ -9578,7 +9586,7 @@
         <v>18000000</v>
       </c>
       <c r="E16" s="15">
-        <f t="shared" ref="E16:K16" si="2">D16-2000000</f>
+        <f t="shared" ref="E16:G16" si="2">D16-2000000</f>
         <v>16000000</v>
       </c>
       <c r="F16" s="15">
@@ -10231,7 +10239,7 @@
         <v>18000000</v>
       </c>
       <c r="E23" s="15">
-        <f t="shared" ref="E23:K23" si="6">D23-2000000</f>
+        <f t="shared" ref="E23:G23" si="6">D23-2000000</f>
         <v>16000000</v>
       </c>
       <c r="F23" s="15">
@@ -11061,7 +11069,7 @@
         <v>18000000</v>
       </c>
       <c r="K29" s="15">
-        <f t="shared" ref="K29:AZ29" si="59">J29-2000000</f>
+        <f t="shared" ref="K29:N29" si="59">J29-2000000</f>
         <v>16000000</v>
       </c>
       <c r="L29" s="15">
@@ -11674,7 +11682,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46CFDA77-5A2D-4C2A-8980-092F1D983A51}">
   <dimension ref="A16:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
@@ -12041,7 +12049,7 @@
         <v>100000</v>
       </c>
       <c r="D35">
-        <f t="shared" ref="D35:G35" si="6">C35</f>
+        <f t="shared" ref="D35:F35" si="6">C35</f>
         <v>100000</v>
       </c>
       <c r="E35">
@@ -12140,7 +12148,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C6E0ACB-123C-4F90-B976-99680DE6121A}">
   <dimension ref="A11:AG21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -12507,8 +12515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E89F9C0D-FB00-40AB-A561-95E189CD5BDE}">
   <dimension ref="A9:K23"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+    <sheetView topLeftCell="A7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12812,8 +12820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEA51B6A-D1ED-406E-88C7-E3A2E2791494}">
   <dimension ref="A11:H35"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12944,7 +12952,7 @@
         <v>16632.000000000004</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="D20:E20" si="0">E13*E14</f>
+        <f t="shared" ref="E20" si="0">E13*E14</f>
         <v>24698.520000000008</v>
       </c>
     </row>
@@ -13975,7 +13983,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{44DCAFAB-475C-4BF5-894E-B0180A6A5BD7}">
   <dimension ref="A10:I30"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -14371,7 +14379,7 @@
   <dimension ref="A8:H12"/>
   <sheetViews>
     <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H12"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14423,7 +14431,7 @@
       <c r="F10">
         <v>10000</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="13">
         <v>0.249999999997427</v>
       </c>
     </row>
@@ -14601,7 +14609,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A808DC9-30B1-460D-B672-8085098FA0B2}">
   <dimension ref="B12:K22"/>
   <sheetViews>
-    <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -14862,7 +14870,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C943F40C-1E57-4A91-BCAB-6FC6B0110466}">
   <dimension ref="A6:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+    <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>